<commit_message>
Add movie_update view to template
</commit_message>
<xml_diff>
--- a/sunghwan_app/static/others/박성환 영화 희망 및 관람 목록.xlsx
+++ b/sunghwan_app/static/others/박성환 영화 희망 및 관람 목록.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-225" yWindow="60" windowWidth="15330" windowHeight="4410" firstSheet="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-225" yWindow="60" windowWidth="15330" windowHeight="4410" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2015년" sheetId="1" r:id="rId1"/>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="217">
   <si>
     <t>박성환 영화 희망목록 및 관람목록</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -875,6 +875,22 @@
   </si>
   <si>
     <t>시각적 상상력의 끝을 보다. 하지만 그게 다다.</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>업</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>피트 닥터, 밥 피터슨</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>가족, 모험</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>적절한 감성, 기발한 상상력. 유쾌해지는 애니메이션.</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -1895,10 +1911,10 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <pane ySplit="4" topLeftCell="A14" activePane="bottomLeft" state="frozenSplit"/>
+    <sheetView workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+      <pane ySplit="4" topLeftCell="A35" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="A17" sqref="A17:XFD18"/>
+      <selection pane="bottomLeft" activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -1925,7 +1941,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="21">
         <f ca="1">NOW()</f>
-        <v>42678.516411111108</v>
+        <v>42681.41199641204</v>
       </c>
       <c r="H1" s="14"/>
     </row>
@@ -2806,10 +2822,10 @@
   </sheetPr>
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
       <pane ySplit="4" topLeftCell="A27" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="D1" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="B6" sqref="B6"/>
+      <selection pane="bottomLeft" activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="24.95" customHeight="1"/>
@@ -2836,7 +2852,7 @@
       <c r="F1" s="31"/>
       <c r="G1" s="21">
         <f ca="1">NOW()</f>
-        <v>42678.516411111108</v>
+        <v>42681.41199641204</v>
       </c>
       <c r="H1" s="14"/>
     </row>
@@ -2852,7 +2868,7 @@
       </c>
       <c r="G2" s="12" t="str">
         <f>COUNTA(A5:A1001)&amp;"편"</f>
-        <v>25편</v>
+        <v>26편</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="3.75" customHeight="1">
@@ -3488,13 +3504,27 @@
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:8" ht="24.95" customHeight="1">
-      <c r="A30" s="15"/>
-      <c r="B30"/>
-      <c r="C30" s="19"/>
-      <c r="D30"/>
-      <c r="E30"/>
-      <c r="F30" s="18"/>
-      <c r="G30" s="17"/>
+      <c r="A30" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B30" t="s">
+        <v>213</v>
+      </c>
+      <c r="C30" s="19" t="s">
+        <v>214</v>
+      </c>
+      <c r="D30" t="s">
+        <v>215</v>
+      </c>
+      <c r="E30" t="s">
+        <v>216</v>
+      </c>
+      <c r="F30" s="18">
+        <v>9</v>
+      </c>
+      <c r="G30" s="17">
+        <v>42680</v>
+      </c>
       <c r="H30" s="6"/>
     </row>
     <row r="31" spans="1:8" ht="24.95" customHeight="1">
@@ -3651,7 +3681,7 @@
       <c r="G1" s="31"/>
       <c r="H1" s="21">
         <f ca="1">NOW()</f>
-        <v>42678.516411111108</v>
+        <v>42681.41199641204</v>
       </c>
       <c r="I1" s="14"/>
     </row>

</xml_diff>